<commit_message>
massive data and figure and script update
update figures/scripts/datasets
</commit_message>
<xml_diff>
--- a/data/Table1.xlsx
+++ b/data/Table1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/peter_regier_pnnl_gov/Documents/Documents/GitHub/peterregier/d50_computer_vision/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{A31A3D3C-8170-5949-A39D-F1A62A0F495A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E763CBF-9907-024D-B7B2-2A95189F6F68}"/>
+  <xr:revisionPtr revIDLastSave="72" documentId="8_{A31A3D3C-8170-5949-A39D-F1A62A0F495A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{367B1D50-CF97-CE4A-AB0B-D7C046A2B10E}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{C2594C85-AAC4-3B42-B9BF-A01B0C3D7F3C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="20">
   <si>
     <t>NEXSS</t>
   </si>
@@ -47,49 +47,55 @@
     <t>YOLO (this study)</t>
   </si>
   <si>
-    <t>Procedure</t>
-  </si>
-  <si>
     <t>Model</t>
   </si>
   <si>
-    <t>Computer vision</t>
-  </si>
-  <si>
     <t>USGS</t>
   </si>
   <si>
     <t>Manual sieving</t>
   </si>
   <si>
-    <t>Range</t>
-  </si>
-  <si>
-    <t>&lt; 2 mm</t>
-  </si>
-  <si>
-    <t>&gt; 2 mm</t>
-  </si>
-  <si>
-    <t>Input variables</t>
-  </si>
-  <si>
-    <t>none</t>
-  </si>
-  <si>
-    <t>KS to add</t>
-  </si>
-  <si>
     <t>Limitations</t>
   </si>
   <si>
-    <t>Model assumptions</t>
-  </si>
-  <si>
-    <t>Misses small or buried particles</t>
-  </si>
-  <si>
-    <t>Misses large particles</t>
+    <t>Spatial extent</t>
+  </si>
+  <si>
+    <t>Inputs</t>
+  </si>
+  <si>
+    <t>images</t>
+  </si>
+  <si>
+    <t>sediments</t>
+  </si>
+  <si>
+    <t>watershed characteristics</t>
+  </si>
+  <si>
+    <t>Model generalizations</t>
+  </si>
+  <si>
+    <t>grains &gt; 2mm</t>
+  </si>
+  <si>
+    <t>Approach</t>
+  </si>
+  <si>
+    <t>point (double-check)</t>
+  </si>
+  <si>
+    <t>reach-scale</t>
+  </si>
+  <si>
+    <t>0.8mx0.8m</t>
+  </si>
+  <si>
+    <t xml:space="preserve">obscured/small (&lt; 2mm) grains </t>
+  </si>
+  <si>
+    <t>Photogrammetry</t>
   </si>
 </sst>
 </file>
@@ -167,7 +173,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -181,13 +187,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -507,96 +516,101 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="E5" sqref="A1:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" customWidth="1"/>
+    <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="5" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5" t="s">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>12</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>10</v>
+      <c r="B5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>9</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E5" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update codes and figures
</commit_message>
<xml_diff>
--- a/data/Table1.xlsx
+++ b/data/Table1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/peter_regier_pnnl_gov/Documents/Documents/GitHub/peterregier/d50_computer_vision/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="8_{A31A3D3C-8170-5949-A39D-F1A62A0F495A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{367B1D50-CF97-CE4A-AB0B-D7C046A2B10E}"/>
+  <xr:revisionPtr revIDLastSave="74" documentId="8_{A31A3D3C-8170-5949-A39D-F1A62A0F495A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E8F33922-7E58-8644-9EA8-15668BAE03E7}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2260" windowWidth="28040" windowHeight="17440" xr2:uid="{C2594C85-AAC4-3B42-B9BF-A01B0C3D7F3C}"/>
   </bookViews>
@@ -41,9 +41,6 @@
     <t>NEXSS</t>
   </si>
   <si>
-    <t>Abeyshu et al. 2022</t>
-  </si>
-  <si>
     <t>YOLO (this study)</t>
   </si>
   <si>
@@ -96,6 +93,9 @@
   </si>
   <si>
     <t>Photogrammetry</t>
+  </si>
+  <si>
+    <t>Abeshu</t>
   </si>
 </sst>
 </file>
@@ -184,7 +184,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -193,10 +193,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -217,7 +217,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -505,7 +505,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -516,7 +516,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="A1:E5"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -530,36 +530,36 @@
   <sheetData>
     <row r="1" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="34" x14ac:dyDescent="0.2">
@@ -567,50 +567,50 @@
         <v>0</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="E3" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>12</v>
-      </c>
       <c r="E4" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="34" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>